<commit_message>
Got Depth Comp Working and Results
</commit_message>
<xml_diff>
--- a/resources/RobustTypesEval.xlsx
+++ b/resources/RobustTypesEval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\playf\OneDrive\Documents\UBC\Thesis\Code\Main_Repo\Alexandre_EyeGaze\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB74F678-8EB5-4093-B22D-21D4CAD9A867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E07A6-1541-4C60-9A69-F2852F0CC385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{021708D6-BD66-47C0-8BE9-F6C3049CC241}"/>
+    <workbookView xWindow="-28800" yWindow="7410" windowWidth="14400" windowHeight="14985" xr2:uid="{021708D6-BD66-47C0-8BE9-F6C3049CC241}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>Function</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>doesn't work well</t>
+  </si>
+  <si>
+    <t>Now with depth compensation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logistic </t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +126,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -215,11 +227,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +272,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +590,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95B5DFA-3E2D-4DD1-B997-D90B6E0CE4DA}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1086,73 +1112,307 @@
       <c r="I18" s="21"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
+      <c r="A19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+    </row>
+    <row r="20" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="D20" s="10">
+        <v>13.0457898189054</v>
+      </c>
+      <c r="E20" s="10">
+        <v>6.3236387726584598</v>
+      </c>
+      <c r="F20" s="9">
+        <v>8.97104068581055</v>
+      </c>
+      <c r="G20" s="11">
+        <v>12.9548253441213</v>
+      </c>
+      <c r="H20" s="10">
+        <v>6.3582802995948704</v>
+      </c>
+      <c r="I20" s="9">
+        <v>7.7346062662048798</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.95898827823361299</v>
+      </c>
+      <c r="K20" s="8">
+        <v>0.92794713448394495</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0.182902536879443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="D21" s="10">
+        <v>13.823196715152999</v>
+      </c>
+      <c r="E21" s="10">
+        <v>6.3711263913771798</v>
+      </c>
+      <c r="F21" s="9">
+        <v>9.4208980160035196</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="8">
+        <v>0.69756692862624903</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0.97601188304499098</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0.176048202921647</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4.6849999999999996</v>
+      </c>
+      <c r="D22" s="4">
+        <v>14.3545490244164</v>
+      </c>
+      <c r="E22" s="4">
+        <v>6.4752167641817397</v>
+      </c>
+      <c r="F22" s="5">
+        <v>9.7026484930519903</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="4"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1.345</v>
+      </c>
+      <c r="D23" s="4">
+        <v>13.8676318191173</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6.3795080709176402</v>
+      </c>
+      <c r="F23" s="5">
+        <v>9.4452931248051293</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>13.5213564398274</v>
+      </c>
+      <c r="E24" s="4">
+        <v>6.3344075811891702</v>
+      </c>
+      <c r="F24" s="5">
+        <v>9.2415788125584992</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="4"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>13.396185506733399</v>
+      </c>
+      <c r="E25" s="4">
+        <v>6.3264555462745697</v>
+      </c>
+      <c r="F25" s="5">
+        <v>9.1695239693596307</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
     </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="24">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>13.300939337265101</v>
+      </c>
+      <c r="E26">
+        <v>6.3249847340029399</v>
+      </c>
+      <c r="F26">
+        <v>9.1175250843445408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="D27">
+        <v>13.2282385224982</v>
+      </c>
+      <c r="E27">
+        <v>6.32344294279787</v>
+      </c>
+      <c r="F27">
+        <v>9.0770030183483499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="24">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>13.1671576402904</v>
+      </c>
+      <c r="E28">
+        <v>6.3232506362195098</v>
+      </c>
+      <c r="F28">
+        <v>9.0434950618111198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>14.179876846369</v>
+      </c>
+      <c r="E29">
+        <v>6.4373665204956003</v>
+      </c>
+      <c r="F29">
+        <v>9.6359162215381904</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>4.2</v>
+      </c>
+      <c r="D31">
+        <v>12.932203298988901</v>
+      </c>
+      <c r="E31">
+        <v>6.3479620377197499</v>
+      </c>
+      <c r="F31">
+        <v>7.7073382190227697</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>12.976867870882201</v>
+      </c>
+      <c r="E32">
+        <v>6.3480426876356804</v>
+      </c>
+      <c r="F32">
+        <v>7.7377683145827101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>1.345</v>
+      </c>
+      <c r="D33">
+        <v>14.337794660389701</v>
+      </c>
+      <c r="E33">
+        <v>6.3440977412476203</v>
+      </c>
+      <c r="F33">
+        <v>8.1354044110535604</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>12.970651546292199</v>
+      </c>
+      <c r="E34">
+        <v>6.3467950776987498</v>
+      </c>
+      <c r="F34">
+        <v>7.7247600078930896</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>